<commit_message>
Richard - Milestone 4 work
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Backlog.xlsx
+++ b/Documentation/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db87de18dbef40e4/Desktop/school/MilestoneProject-git/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{F4E2009E-C777-4B40-872E-F910BCCB6E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A5CD3CB8-FC66-4FF8-89D5-53E013E6195A}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{F4E2009E-C777-4B40-872E-F910BCCB6E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7671DB6F-8C35-45F0-87FC-F7D25A01336E}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2798" windowWidth="21600" windowHeight="11422" xr2:uid="{10A44738-0BFE-40BF-939A-D4346DBDDC88}"/>
+    <workbookView xWindow="2858" yWindow="2520" windowWidth="21600" windowHeight="11423" xr2:uid="{10A44738-0BFE-40BF-939A-D4346DBDDC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
   <si>
     <t>Milestone</t>
   </si>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754CB959-AF8B-494D-8684-AB937015E3F6}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -659,6 +659,7 @@
     <col min="1" max="1" width="11.1328125" customWidth="1"/>
     <col min="2" max="2" width="58.59765625" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -934,7 +935,12 @@
       <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="D20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="7">
+        <v>44339</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
@@ -943,7 +949,12 @@
       <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
@@ -952,7 +963,12 @@
       <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
@@ -961,7 +977,12 @@
       <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
@@ -971,8 +992,12 @@
         <v>15</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="9">
+        <v>44339</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">

</xml_diff>

<commit_message>
Richard doing the things for MILESTONE 5, product update, edit delete, and search
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Backlog.xlsx
+++ b/Documentation/Sprint Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db87de18dbef40e4/Desktop/school/MilestoneProject-git/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="8_{F4E2009E-C777-4B40-872E-F910BCCB6E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7671DB6F-8C35-45F0-87FC-F7D25A01336E}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{F4E2009E-C777-4B40-872E-F910BCCB6E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF12B469-BF5E-4304-92A2-98E6D69674BD}"/>
   <bookViews>
-    <workbookView xWindow="2858" yWindow="2520" windowWidth="21600" windowHeight="11423" xr2:uid="{10A44738-0BFE-40BF-939A-D4346DBDDC88}"/>
+    <workbookView xWindow="285" yWindow="4178" windowWidth="21600" windowHeight="11422" xr2:uid="{10A44738-0BFE-40BF-939A-D4346DBDDC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="62">
   <si>
     <t>Milestone</t>
   </si>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754CB959-AF8B-494D-8684-AB937015E3F6}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1006,7 +1006,12 @@
       <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
@@ -1015,7 +1020,12 @@
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="D26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
@@ -1024,7 +1034,12 @@
       <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="D27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
@@ -1033,7 +1048,12 @@
       <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="D28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
@@ -1042,7 +1062,12 @@
       <c r="B29" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
@@ -1051,7 +1076,12 @@
       <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="D30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
@@ -1061,8 +1091,12 @@
         <v>15</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="8"/>
+      <c r="D31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
@@ -1072,8 +1106,12 @@
         <v>40</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="10"/>
+      <c r="D32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="7">
+        <v>44346</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">

</xml_diff>

<commit_message>
Richard adding JQuery to home for listing and searching products, uses AJAX
</commit_message>
<xml_diff>
--- a/Documentation/Sprint Backlog.xlsx
+++ b/Documentation/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db87de18dbef40e4/Desktop/school/MilestoneProject-git/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="8_{F4E2009E-C777-4B40-872E-F910BCCB6E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF12B469-BF5E-4304-92A2-98E6D69674BD}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{F4E2009E-C777-4B40-872E-F910BCCB6E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF95516-F4C2-4E96-B99A-CE10F415386C}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="4178" windowWidth="21600" windowHeight="11422" xr2:uid="{10A44738-0BFE-40BF-939A-D4346DBDDC88}"/>
+    <workbookView xWindow="0" yWindow="1245" windowWidth="21600" windowHeight="11423" xr2:uid="{10A44738-0BFE-40BF-939A-D4346DBDDC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="63">
   <si>
     <t>Milestone</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Misty</t>
+  </si>
+  <si>
+    <t>6/6/20201</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1109,7 +1112,7 @@
       <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="9">
         <v>44346</v>
       </c>
     </row>
@@ -1120,7 +1123,12 @@
       <c r="B33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">

</xml_diff>